<commit_message>
data imported through external file
</commit_message>
<xml_diff>
--- a/meta_info.xlsx
+++ b/meta_info.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tausif\node-react-crud\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shopify-rest-api\node-shopify-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="meta_info" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -865,23 +865,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>6902262300808</v>
       </c>
@@ -921,7 +921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>6907111145609</v>
       </c>
@@ -938,6 +938,46 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>6907111145609</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>6907111145609</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>